<commit_message>
convert from bool to int for one-hot encoding
</commit_message>
<xml_diff>
--- a/scores/f_stats_score.xlsx
+++ b/scores/f_stats_score.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>480501.5940585519</v>
+        <v>480501.5940585432</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -465,7 +465,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>455370.5074818575</v>
+        <v>455370.5074817779</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
@@ -478,7 +478,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>430547.7518363342</v>
+        <v>430547.7518362895</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -491,7 +491,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>386536.7962757756</v>
+        <v>386536.796275733</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -504,7 +504,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>383419.9165281194</v>
+        <v>383419.9165281813</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
@@ -517,7 +517,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>381544.4216970277</v>
+        <v>381544.421696993</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
@@ -530,7 +530,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>360089.6806642293</v>
+        <v>360089.6806646097</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
@@ -543,7 +543,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>351038.5261179841</v>
+        <v>351038.5261179415</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
@@ -556,7 +556,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>314046.745169116</v>
+        <v>314046.7451691181</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
@@ -647,7 +647,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>119297.4733137381</v>
+        <v>119297.4733137136</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
@@ -920,7 +920,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>13976.39007839663</v>
+        <v>13976.39007832004</v>
       </c>
       <c r="C38" t="n">
         <v>0</v>
@@ -1063,7 +1063,7 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>3522.866232951488</v>
+        <v>3522.866232955121</v>
       </c>
       <c r="C49" t="n">
         <v>0</v>
@@ -1206,10 +1206,10 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>557.7422474310656</v>
+        <v>557.7422474402912</v>
       </c>
       <c r="C60" t="n">
-        <v>3.152567504874911e-123</v>
+        <v>3.152567490388702e-123</v>
       </c>
     </row>
     <row r="61">
@@ -1245,10 +1245,10 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>86.23438165503438</v>
+        <v>86.23438164615078</v>
       </c>
       <c r="C63" t="n">
-        <v>1.605705116807071e-20</v>
+        <v>1.605705124063689e-20</v>
       </c>
     </row>
     <row r="64">

</xml_diff>

<commit_message>
change the target variable to R_TEMP + regression tree
</commit_message>
<xml_diff>
--- a/scores/f_stats_score.xlsx
+++ b/scores/f_stats_score.xlsx
@@ -448,11 +448,11 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>R_O2</t>
+          <t>R_SVA</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>399327.0488132559</v>
+        <v>2714888.40129829</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -465,7 +465,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>358875.191427839</v>
+        <v>2684356.106899888</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
@@ -474,11 +474,11 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>R_O2_sqrt</t>
+          <t>R_DYNHT</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>358025.5032421126</v>
+        <v>530519.5946675759</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -487,11 +487,11 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>R_SVA</t>
+          <t>R_O2Sat</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>350012.6979454875</v>
+        <v>396759.2753411022</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -500,11 +500,11 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>R_O2Sat</t>
+          <t>R_O2</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>342162.0020536334</v>
+        <v>323055.8579581335</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
@@ -513,11 +513,11 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>R_DYNHT</t>
+          <t>R_Depth</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>305379.7525019657</v>
+        <v>312594.9482566265</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
@@ -526,11 +526,11 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>R_PRES_cat_(237.5, inf]</t>
+          <t>R_PRES</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>248887.9830678838</v>
+        <v>310283.4061970197</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
@@ -539,11 +539,11 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>R_Depth_cat_(0.5, 95.5]</t>
+          <t>R_O2_sqrt</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>220370.0891608632</v>
+        <v>277008.4668065083</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
@@ -552,11 +552,11 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>R_PRES_cat_(0.0, 95.5]</t>
+          <t>R_PRES_cat_(317.5, inf]</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>220302.8353846216</v>
+        <v>249871.3379890129</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
@@ -565,11 +565,11 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>R_Depth</t>
+          <t>R_PO4</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>193820.4697281373</v>
+        <v>188769.7217200231</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
@@ -578,11 +578,11 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>R_PRES</t>
+          <t>R_PRES_cat_(0.0, 47.5]</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>192604.3182522946</v>
+        <v>186582.6372257432</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
@@ -591,11 +591,11 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>R_PO4</t>
+          <t>R_NO3</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>152820.9161675356</v>
+        <v>135301.1896482321</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
@@ -604,11 +604,11 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>R_PO4_cat_(0.0, 1.305]</t>
+          <t>R_Depth_cat_(315.5, 671.5]</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>133331.1733469558</v>
+        <v>114797.8075130635</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
@@ -617,11 +617,11 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>R_NO3</t>
+          <t>R_SALINITY</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>128027.8682686344</v>
+        <v>102144.5845694863</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
@@ -630,11 +630,11 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>R_TEMP</t>
+          <t>R_SIO3</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>120469.5396235875</v>
+        <v>101280.6243001091</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
@@ -643,11 +643,11 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>R_SIO3_cat_(0.0, 12.75]</t>
+          <t>R_PO4_cat_(0.0, 0.505]</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>119103.1331728772</v>
+        <v>98325.81600348902</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
@@ -656,11 +656,11 @@
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>R_CHLA_cat_(0.055, 1.225]</t>
+          <t>R_SIO3_cat_(0.0, 3.55]</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>110768.0411033612</v>
+        <v>77322.10248279784</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
@@ -669,11 +669,11 @@
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>R_Depth_cat_(284.5, 648.5]</t>
+          <t>R_Depth_cat_(0.0, 15.5]</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>106597.4428800327</v>
+        <v>70912.69712999069</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
@@ -682,11 +682,11 @@
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>R_CHLA_missing</t>
+          <t>R_Depth_cat_(671.5, inf]</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>91118.98443980375</v>
+        <v>59855.32231765103</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
@@ -695,11 +695,11 @@
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>R_PHAEO_missing</t>
+          <t>R_Depth_cat_(15.5, 47.5]</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>91073.74676871888</v>
+        <v>58327.66354584995</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
@@ -708,11 +708,11 @@
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>R_SIO3</t>
+          <t>R_CHLA_cat_(0.065, inf]</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>83713.35372309758</v>
+        <v>57300.55019632763</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
@@ -721,11 +721,11 @@
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>R_NO3_cat_(0.0, 13.05]</t>
+          <t>R_PO4_cat_(2.505, inf]</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>70047.16134946943</v>
+        <v>54652.06555948611</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
@@ -734,11 +734,11 @@
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>Lat_Dec</t>
+          <t>R_SIO3_cat_(42.05, inf]</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>56008.64519927528</v>
+        <v>44579.70349106604</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
@@ -747,11 +747,11 @@
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>R_PHAEO_cat_(0.095, 1.395]</t>
+          <t>R_NO3_cat_(30.05, inf]</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>55450.78207401488</v>
+        <v>42233.56007720197</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
@@ -760,11 +760,11 @@
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>R_PO4_cat_(2.305, inf]</t>
+          <t>R_CHLA_missing</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>52466.698535603</v>
+        <v>29910.27770914006</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
@@ -773,11 +773,11 @@
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>Phi</t>
+          <t>R_PHAEO_missing</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>45484.72160684083</v>
+        <v>29887.44598188028</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
@@ -786,11 +786,11 @@
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>Rho</t>
+          <t>R_NO3_cat_(0.0, 0.55]</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>43730.44773022123</v>
+        <v>26783.15453731845</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
@@ -799,11 +799,11 @@
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>R_SIO3_cat_(34.95, inf]</t>
+          <t>R_PRES_cat_(118.5, 317.5]</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>41658.44722556435</v>
+        <v>26715.03066051535</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
@@ -812,11 +812,11 @@
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>R_Depth_cat_(648.5, inf]</t>
+          <t>R_Depth_cat_(167.5, 315.5]</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>41427.27099051326</v>
+        <v>25822.77443068063</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
@@ -825,11 +825,11 @@
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>R_NO3_cat_(27.15, inf]</t>
+          <t>Lat_Dec</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>36477.85928166637</v>
+        <v>24458.4687073659</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
@@ -838,11 +838,11 @@
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>Lon_Dec</t>
+          <t>Phi</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>35267.41162643352</v>
+        <v>21039.15155552508</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
@@ -851,11 +851,11 @@
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>R_Depth_cat_(183.5, 284.5]</t>
+          <t>R_PRES_cat_(47.5, 118.5]</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>24732.79715979379</v>
+        <v>16902.02769188509</v>
       </c>
       <c r="C33" t="n">
         <v>0</v>
@@ -864,11 +864,11 @@
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>R_NO2_cat_(0.055, inf]</t>
+          <t>Rho</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>20622.08853197142</v>
+        <v>16370.32515075266</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
@@ -877,11 +877,11 @@
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>R_NO2_missing</t>
+          <t>R_Depth_cat_(47.5, 68.5]</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>17426.83809469752</v>
+        <v>13972.79318691749</v>
       </c>
       <c r="C35" t="n">
         <v>0</v>
@@ -890,11 +890,11 @@
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>R_NO3_missing</t>
+          <t>Lon_Dec</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>16481.43488930288</v>
+        <v>12528.24531616173</v>
       </c>
       <c r="C36" t="n">
         <v>0</v>
@@ -903,11 +903,11 @@
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>R_SIO3_missing</t>
+          <t>R_PHAEO_cat_(0.015, 0.175]</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>16378.05375755484</v>
+        <v>12332.20428891879</v>
       </c>
       <c r="C37" t="n">
         <v>0</v>
@@ -916,11 +916,11 @@
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>R_PO4_missing</t>
+          <t>R_PHAEO_cat_(0.175, inf]</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>13766.05517659665</v>
+        <v>9823.414394576244</v>
       </c>
       <c r="C38" t="n">
         <v>0</v>
@@ -929,11 +929,11 @@
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>R_PRES_cat_(148.5, 237.5]</t>
+          <t>R_PO4_cat_(1.025, 2.505]</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>12338.62598943843</v>
+        <v>8483.247546078766</v>
       </c>
       <c r="C39" t="n">
         <v>0</v>
@@ -942,11 +942,11 @@
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>R_PHAEO_cat_(0.0, 0.065]</t>
+          <t>R_NO3_cat_(0.55, 10.85]</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>10784.26111476153</v>
+        <v>7144.489441342773</v>
       </c>
       <c r="C40" t="n">
         <v>0</v>
@@ -955,11 +955,11 @@
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>R_NO2</t>
+          <t>R_SIO3_cat_(3.55, 10.05]</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>7299.08508152496</v>
+        <v>6592.698967501911</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
@@ -968,11 +968,11 @@
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>R_PHAEO_cat_(0.065, 0.095]</t>
+          <t>R_PO4_cat_(0.505, 1.025]</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>5009.748733283909</v>
+        <v>6276.513287597355</v>
       </c>
       <c r="C42" t="n">
         <v>0</v>
@@ -981,11 +981,11 @@
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>R_NH4_cat_(0.045, inf]</t>
+          <t>R_NO3_cat_(10.85, 30.05]</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>4814.048826474694</v>
+        <v>4969.737007009157</v>
       </c>
       <c r="C43" t="n">
         <v>0</v>
@@ -994,11 +994,11 @@
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>R_NO3_cat_(13.05, 20.95]</t>
+          <t>R_NO2_cat_(0.045, 1.665]</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>4380.938543579192</v>
+        <v>4756.664337434716</v>
       </c>
       <c r="C44" t="n">
         <v>0</v>
@@ -1007,11 +1007,11 @@
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>R_NH4_missing</t>
+          <t>R_SIO3_cat_(10.05, 42.05]</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>4335.702481166432</v>
+        <v>4663.385373806259</v>
       </c>
       <c r="C45" t="n">
         <v>0</v>
@@ -1020,11 +1020,11 @@
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>R_SIO3_cat_(12.75, 22.95]</t>
+          <t>R_CHLA</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>4187.606362793627</v>
+        <v>3814.564890351276</v>
       </c>
       <c r="C46" t="n">
         <v>0</v>
@@ -1033,11 +1033,11 @@
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>R_NO2_cat_(0.025, 0.055]</t>
+          <t>R_Depth_cat_(68.5, 117.5]</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>3663.444142144021</v>
+        <v>3546.943169601435</v>
       </c>
       <c r="C47" t="n">
         <v>0</v>
@@ -1046,11 +1046,11 @@
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>R_Depth_cat_(95.5, 115.5]</t>
+          <t>R_PHAEO_cat_(0.005, 0.015]</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>3559.230803380447</v>
+        <v>1967.627482069903</v>
       </c>
       <c r="C48" t="n">
         <v>0</v>
@@ -1059,11 +1059,11 @@
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>R_CHLA</t>
+          <t>R_NH4_cat_(0.045, inf]</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>3491.979077141535</v>
+        <v>1591.697259690214</v>
       </c>
       <c r="C49" t="n">
         <v>0</v>
@@ -1072,11 +1072,11 @@
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>R_CHLA_cat_(1.225, inf]</t>
+          <t>R_PHAEO</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>3389.284615899776</v>
+        <v>1572.4400613119</v>
       </c>
       <c r="C50" t="n">
         <v>0</v>
@@ -1085,11 +1085,11 @@
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>R_PO4_cat_(1.745, 2.305]</t>
+          <t>R_NO2</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>2894.164220893094</v>
+        <v>1551.306333968829</v>
       </c>
       <c r="C51" t="n">
         <v>0</v>
@@ -1098,92 +1098,92 @@
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>R_PHAEO</t>
+          <t>R_Depth_cat_(117.5, 167.5]</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>2840.530483982403</v>
+        <v>1412.670400904832</v>
       </c>
       <c r="C52" t="n">
-        <v>0</v>
+        <v>1.422076229348544e-308</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>R_PRES_cat_(95.5, 148.5]</t>
+          <t>R_NO2_missing</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>2719.430384119639</v>
+        <v>1397.864526552771</v>
       </c>
       <c r="C53" t="n">
-        <v>0</v>
+        <v>2.280935432565034e-305</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>R_PO4_cat_(1.305, 1.745]</t>
+          <t>R_CHLA_cat_(0.0, 0.015]</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>2679.95695576749</v>
+        <v>1320.503532934729</v>
       </c>
       <c r="C54" t="n">
-        <v>0</v>
+        <v>1.281670447809801e-288</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>R_Depth_cat_(147.5, 183.5]</t>
+          <t>R_SIO3_missing</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>1924.060380502762</v>
+        <v>1296.262630684214</v>
       </c>
       <c r="C55" t="n">
-        <v>0</v>
+        <v>2.275688171524229e-283</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>R_NH4_cat_(0.005, 0.045]</t>
+          <t>R_PO4_missing</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>1302.47705262344</v>
+        <v>655.2476995483604</v>
       </c>
       <c r="C56" t="n">
-        <v>9.238096750754673e-285</v>
+        <v>2.15686008779483e-144</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>R_NH4</t>
+          <t>R_NO3_missing</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>1176.454148799718</v>
+        <v>569.8346465847553</v>
       </c>
       <c r="C57" t="n">
-        <v>1.863446509647639e-257</v>
+        <v>7.596557236730098e-126</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
-          <t>R_SIO3_cat_(22.95, 34.95]</t>
+          <t>R_NO2_cat_(0.005, 0.045]</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>1146.095015377207</v>
+        <v>555.84655807102</v>
       </c>
       <c r="C58" t="n">
-        <v>7.0742666375706e-251</v>
+        <v>8.295775193515382e-123</v>
       </c>
     </row>
     <row r="59">
@@ -1193,94 +1193,94 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>825.3894916569974</v>
+        <v>469.3354099914836</v>
       </c>
       <c r="C59" t="n">
-        <v>2.473512213217385e-181</v>
+        <v>5.189420311970072e-104</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
         <is>
-          <t>R_NO2_cat_(0.015, 0.025]</t>
+          <t>R_NH4</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>775.3490492612954</v>
+        <v>464.6456392323434</v>
       </c>
       <c r="C60" t="n">
-        <v>1.78537246390994e-170</v>
+        <v>5.424718510009815e-103</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
         <is>
-          <t>R_NO3_cat_(20.95, 27.15]</t>
+          <t>R_NH4_cat_(0.005, 0.045]</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>671.9978934370414</v>
+        <v>155.721508817497</v>
       </c>
       <c r="C61" t="n">
-        <v>4.845978129668273e-148</v>
+        <v>9.901815599470554e-36</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
         <is>
-          <t>R_Depth_cat_(115.5, 147.5]</t>
+          <t>R_CHLA_cat_(0.055, 0.065]</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>193.3367544906929</v>
+        <v>152.0199182661288</v>
       </c>
       <c r="C62" t="n">
-        <v>6.082147870135203e-44</v>
+        <v>6.372760923046343e-35</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
         <is>
-          <t>R_CHLA_cat_(0.0, 0.015]</t>
+          <t>R_NH4_missing</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>130.9109130646468</v>
+        <v>144.6229425417114</v>
       </c>
       <c r="C63" t="n">
-        <v>2.617434340511192e-30</v>
+        <v>2.633928854950761e-33</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
         <is>
-          <t>R_PHAEO_cat_(1.395, inf]</t>
+          <t>R_NO2_cat_(1.665, inf]</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>31.30123369936086</v>
+        <v>24.16611469822136</v>
       </c>
       <c r="C64" t="n">
-        <v>2.210800816309382e-08</v>
+        <v>8.841122614622893e-07</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
-          <t>R_NO2_cat_(0.0, 0.015]</t>
+          <t>R_PHAEO_cat_(0.0, 0.005]</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>8.705254727007112</v>
+        <v>0</v>
       </c>
       <c r="C65" t="n">
-        <v>0.003173120762919951</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
         <is>
-          <t>R_Depth_missing</t>
+          <t>R_NH4_cat_(0.0, 0.005]</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -1293,7 +1293,7 @@
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
         <is>
-          <t>R_PRES_missing</t>
+          <t>R_Depth_missing</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -1306,7 +1306,7 @@
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
         <is>
-          <t>R_Depth_cat_(0.0, 0.5]</t>
+          <t>R_PRES_missing</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -1319,7 +1319,7 @@
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
         <is>
-          <t>R_NH4_cat_(0.0, 0.005]</t>
+          <t>R_NO2_cat_(0.0, 0.005]</t>
         </is>
       </c>
       <c r="B69" t="n">

</xml_diff>